<commit_message>
Update visualisation with updated data
</commit_message>
<xml_diff>
--- a/eval_visualisations/Bert-scores-visualisation.xlsx
+++ b/eval_visualisations/Bert-scores-visualisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul Sharma\OneDrive - UWA\UWA\Sem_3_Capstone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3DC4BA-44B1-4FD3-B993-8892643D4BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0DDE0-078F-44CC-9ADA-208636581C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{5A277C85-1EFA-480F-A9F1-FAE903B22EB9}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$256</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="526">
   <si>
     <t>FILENAME</t>
   </si>
@@ -1532,9 +1532,6 @@
     <t>llama 3.2</t>
   </si>
   <si>
-    <t>Nicolls-Diver-Finding</t>
-  </si>
-  <si>
     <t>The deceased were: Ruby Natasha Nicholls-Diver, Carly Jean Elliott, Michael Ronald Thomas, Anthony Ian Edwards, Stephen Colin Robson</t>
   </si>
   <si>
@@ -1903,9 +1900,6 @@
 The case demonstrates how missed opportunities can occur in situations where institutions or individuals fail to fully address concerns raised by family members or other parties involved with a child's care. It suggests that even with proper procedures and policies in place, failure to follow through on those procedures can still result in negative outcomes.
 Furthermore, the tragic death of Baby H highlights the importance of effective communication among different stakeholders involved in a child's care, as well as the need for swift action when concerns are raised about a child's welfare. The fact that some opportunities to intervene were missed due to delays or lack of coordination between agencies emphasizes the need for improved coordination and follow-up procedures.
 Overall, this case underscores the importance of rigorous implementation of new practice guides and rules in institutions like the Department, as well as the need for continuous improvement and lessons learned from cases like Baby H's.</t>
-  </si>
-  <si>
-    <t>Forkin_finding_2014</t>
   </si>
   <si>
     <t>The deceased's name has been omitted in your provided text; hence I cannot directly identify it from this specific excerpt alone without additional contextual clues or details that usually accompany such descriptions (e.g., a birth certificate would confirm his first and last names).</t>
@@ -2390,6 +2384,52 @@
   </si>
   <si>
     <t>0.8507838249206543</t>
+  </si>
+  <si>
+    <t>Yes. The Rodier case underscores a broader public safety lesson about the persistent dangers of rock fishing and the need for preventive measures at hazardous coastal sites. The coroner observed that while Western Australia has since introduced safety improvements such as life rings and tether points at popular rock fishing locations, remote areas like Quobba Station remain perilous and largely unmonitored. The finding highlights how environmental risks, rather than institutional failures, were central, emphasizing the importance of sustained public education, signage, and infrastructure to reduce fatalities from recreational fishing accidents</t>
+  </si>
+  <si>
+    <t>Yes, this case highlights several broader patterns and lessons relevant to public safety and institutional care. Some of these include:
+1. The importance of thorough and timely investigations into missing persons cases: The fact that Frank's disappearance was not initially treated as a suspicious death until 2023 suggests that there may have been missed opportunities for investigation or communication with the family.
+2. The need for effective communication between law enforcement agencies, coroners' offices, and families: The case involved multiple reviews of Frank's disappearance over several decades, with different outcomes at each stage. This highlights the importance of clear communication and coordination across these organizations to ensure that cases are handled appropriately.
+3. The impact of institutional failures on individual safety: Frank's death appears to have been the result of a combination of factors, including his age, health status, and likely lack of supervision while out in the community. This suggests that older adults or vulnerable populations may be disproportionately affected by institutional failures.
+4. The role of coroners' inquiries in ensuring public safety: As Acting State Coroner, the author of the decision played a crucial role in investigating Frank's death and identifying potential causes. This highlights the importance of coroners' offices in holding institutions accountable for their actions and ensuring that lessons are learned from tragic events.
+5. The need for ongoing support and resources for families affected by missing persons cases: The case involved multiple reviews over several decades, with no resolution until 2023. This suggests that families may require ongoing support and resources to cope with the uncertainty and lack of closure that can accompany a missing person's case.</t>
+  </si>
+  <si>
+    <t>Based on the provided context information, it appears that the coroner did not make any explicit recommendations for future prevention. The text states that the coroner "did not address those general issues separately from a consideration of each death" and that many of the systemic issues mentioned in evidence were not sufficiently connected to all the respective deaths for the coroner to comment on them.
+However, it can be inferred that the coroner did make some recommendations based on the context information provided. The text mentions that the evidence related to general or systemic issues pertinent to Graylands was adduced "to investigate whether those issues had bearing on any or some of the deaths" and to allow the Court to comment on the quality of supervision, treatment, and care of the deceased patients.
+The fact that evidence regarding the condition of the buildings at Graylands was provided suggests that the coroner may have made recommendations related to environmental or physical conditions. The text states that "the physical environment of the wards would have been more therapeutic had the buildings been refurbished," which implies that the coroner considered the potential impact of these environmental factors on the treatment and care of patients.
+Overall, while the text does not explicitly state the coroner's recommendations for future prevention, it suggests that the coroner did consider systemic issues related to Graylands and may have made implicit recommendations for improvement in this regard.</t>
+  </si>
+  <si>
+    <t>Immediate cause: Ligature compression of the neck (hanging) (page 14). Contributing factors: Substance abuse, personality disorder, pending court case, strained relationship with his mother, and recent absconding from psychiatric care (pages 9–13, 20)</t>
+  </si>
+  <si>
+    <t>Based on the provided context information, the immediate cause of death is ligature compression of the neck (hanging), as concluded by Chief Forensic Pathologist Dr. C T Cooke.
+The contributing factors that led to the hanging include:
+1. The unlocked front door, which allowed unauthorized access to the house.
+2. The electrical cord tied to a rafter through an open manhole in the ceiling, providing a means for the deceased to hang himself.
+3. The use of cannabis within 24 hours, as indicated by a low level of tetrahydrocannabinol, may have impaired judgment and increased the risk of suicidal behavior.
+It's worth noting that these contributing factors did not directly cause the death, but rather provided the circumstances in which the hanging occurred.</t>
+  </si>
+  <si>
+    <t>Based on the provided context information, it appears that the coroner did address some aspects of the quality of supervision, treatment, and care provided to the deceased. The relevant excerpts suggest that:
+1. The coroner considered general evidence related to systemic issues at Graylands, but determined that many of these issues were not sufficiently connected to each individual death to warrant comment under s.25.
+2. The coroner did evaluate the risk assessment and decision-making process surrounding the deceased's unescorted ground access, concluding that there was no reasonable basis for criticism.
+3. The coroner also considered the treating team's approach to treatment and acknowledged that there were legitimate criticisms if the treatment had been more restrictive.
+However, it is not explicitly stated whether the coroner evaluated the adequacy of supervision, treatment, or care provided in a comprehensive manner, taking into account each individual death. The excerpts suggest that the coroner's evaluation was context-dependent, focusing on specific aspects and connections to individual deaths rather than providing a broad assessment of the overall quality of care.
+In summary, while the coroner did evaluate certain aspects of supervision, treatment, and care, it is unclear whether this evaluation was comprehensive or solely focused on specific issues connected to individual deaths.</t>
+  </si>
+  <si>
+    <t>Yes, this case highlights several broader patterns and lessons relevant to public safety and institutional care. Here are a few:
+1. **Inadequate supervision and risk management**: The fact that the deceased was able to abscond from Graylands twice (on November 29th and December 7th) raises concerns about the effectiveness of the institution's supervision and risk management systems. This suggests that the institution may not have been adequately prepared to prevent or respond to such incidents.
+2. **Lack of adequate care planning**: The deceased's aggressive behavior, suicidal tendencies, and history of manipulating the system for his gratification suggest that he required more intensive and specialized care than was likely provided at Graylands. This highlights the importance of having adequate care plans in place for patients with complex needs.
+3. **Inadequate record-keeping and communication**: The lack of proper record-keeping of the deceased's ground access, as well as delays in declaring him AWOL after his second absconding, suggest that there were communication breakdowns between staff members and potentially between institutions.
+4. **Need for improved treatment approaches**: The fact that the deceased was able to manipulate the system to achieve his goals, despite being a "difficult patient," suggests that traditional treatment approaches may not be effective in managing complex mental health conditions.
+5. **Importance of adequate staffing ratios and training**: The incident highlights the need for adequate staffing ratios and training for staff members who work with patients with high-risk behaviors. This is particularly important in institutions where patients may pose a risk to themselves or others.
+6. **Need for better coordination between institutions**: The fact that the deceased was able to abscond twice, despite being on a suspended sentence of imprisonment, suggests that there may be gaps in communication and coordination between Graylands and other institutions involved in his care.
+These broader patterns and lessons highlight the need for improved institutional care, supervision, and risk management systems, as well as more effective treatment approaches and better communication and coordination between institutions.</t>
   </si>
 </sst>
 </file>
@@ -2471,7 +2511,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2801,10 +2882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0490D49-417E-4222-A93E-5008B1C77A87}">
-  <dimension ref="A1:H251"/>
+  <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C247" sqref="C247"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3627,7 +3708,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D32" t="s">
         <v>90</v>
@@ -3653,7 +3734,7 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D33" t="s">
         <v>92</v>
@@ -3679,7 +3760,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D34" t="s">
         <v>94</v>
@@ -3705,7 +3786,7 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D35" t="s">
         <v>96</v>
@@ -3731,7 +3812,7 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D36" t="s">
         <v>98</v>
@@ -3757,7 +3838,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D37" t="s">
         <v>100</v>
@@ -3783,7 +3864,7 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D38" t="s">
         <v>102</v>
@@ -3809,7 +3890,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D39" t="s">
         <v>104</v>
@@ -3835,7 +3916,7 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D40" t="s">
         <v>106</v>
@@ -6975,7 +7056,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B161" t="s">
         <v>331</v>
@@ -6984,10 +7065,10 @@
         <v>10</v>
       </c>
       <c r="D161" t="s">
+        <v>332</v>
+      </c>
+      <c r="E161" t="s">
         <v>333</v>
-      </c>
-      <c r="E161" t="s">
-        <v>334</v>
       </c>
       <c r="F161">
         <v>0.88972711563110352</v>
@@ -7001,19 +7082,19 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B162" t="s">
         <v>331</v>
       </c>
       <c r="C162" t="s">
-        <v>335</v>
+        <v>13</v>
       </c>
       <c r="D162" t="s">
         <v>144</v>
       </c>
       <c r="E162" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F162">
         <v>0.8679928183555603</v>
@@ -7027,19 +7108,19 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B163" t="s">
         <v>331</v>
       </c>
       <c r="C163" t="s">
-        <v>337</v>
+        <v>16</v>
       </c>
       <c r="D163" t="s">
         <v>146</v>
       </c>
       <c r="E163" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F163">
         <v>0.87599444389343262</v>
@@ -7053,7 +7134,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B164" t="s">
         <v>331</v>
@@ -7065,7 +7146,7 @@
         <v>148</v>
       </c>
       <c r="E164" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F164">
         <v>0.81340193748474121</v>
@@ -7079,7 +7160,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B165" t="s">
         <v>331</v>
@@ -7091,7 +7172,7 @@
         <v>150</v>
       </c>
       <c r="E165" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F165">
         <v>0.80352234840393066</v>
@@ -7105,7 +7186,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B166" t="s">
         <v>331</v>
@@ -7114,10 +7195,10 @@
         <v>25</v>
       </c>
       <c r="D166" t="s">
+        <v>340</v>
+      </c>
+      <c r="E166" t="s">
         <v>341</v>
-      </c>
-      <c r="E166" t="s">
-        <v>342</v>
       </c>
       <c r="F166">
         <v>0.84147226810455322</v>
@@ -7131,7 +7212,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B167" t="s">
         <v>331</v>
@@ -7140,10 +7221,10 @@
         <v>28</v>
       </c>
       <c r="D167" t="s">
+        <v>342</v>
+      </c>
+      <c r="E167" t="s">
         <v>343</v>
-      </c>
-      <c r="E167" t="s">
-        <v>344</v>
       </c>
       <c r="F167">
         <v>0.83174103498458862</v>
@@ -7157,7 +7238,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B168" t="s">
         <v>331</v>
@@ -7166,10 +7247,10 @@
         <v>37</v>
       </c>
       <c r="D168" t="s">
+        <v>344</v>
+      </c>
+      <c r="E168" t="s">
         <v>345</v>
-      </c>
-      <c r="E168" t="s">
-        <v>346</v>
       </c>
       <c r="F168">
         <v>0.82274585962295532</v>
@@ -7183,7 +7264,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B169" t="s">
         <v>331</v>
@@ -7192,10 +7273,10 @@
         <v>31</v>
       </c>
       <c r="D169" t="s">
+        <v>346</v>
+      </c>
+      <c r="E169" t="s">
         <v>347</v>
-      </c>
-      <c r="E169" t="s">
-        <v>348</v>
       </c>
       <c r="F169">
         <v>0.80642694234848022</v>
@@ -7209,7 +7290,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B170" t="s">
         <v>331</v>
@@ -7218,10 +7299,10 @@
         <v>34</v>
       </c>
       <c r="D170" t="s">
+        <v>348</v>
+      </c>
+      <c r="E170" t="s">
         <v>349</v>
-      </c>
-      <c r="E170" t="s">
-        <v>350</v>
       </c>
       <c r="F170">
         <v>0.83886325359344482</v>
@@ -7235,7 +7316,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B171" t="s">
         <v>331</v>
@@ -7247,7 +7328,7 @@
         <v>191</v>
       </c>
       <c r="E171" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F171">
         <v>0.86437129974365234</v>
@@ -7261,7 +7342,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B172" t="s">
         <v>331</v>
@@ -7270,10 +7351,10 @@
         <v>43</v>
       </c>
       <c r="D172" t="s">
+        <v>351</v>
+      </c>
+      <c r="E172" t="s">
         <v>352</v>
-      </c>
-      <c r="E172" t="s">
-        <v>353</v>
       </c>
       <c r="F172">
         <v>0.83225011825561523</v>
@@ -7287,7 +7368,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B173" t="s">
         <v>331</v>
@@ -7296,10 +7377,10 @@
         <v>46</v>
       </c>
       <c r="D173" t="s">
+        <v>353</v>
+      </c>
+      <c r="E173" t="s">
         <v>354</v>
-      </c>
-      <c r="E173" t="s">
-        <v>355</v>
       </c>
       <c r="F173">
         <v>0.81613105535507202</v>
@@ -7313,7 +7394,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B174" t="s">
         <v>331</v>
@@ -7325,7 +7406,7 @@
         <v>197</v>
       </c>
       <c r="E174" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F174">
         <v>0.85510623455047607</v>
@@ -7339,7 +7420,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>332</v>
+        <v>174</v>
       </c>
       <c r="B175" t="s">
         <v>331</v>
@@ -7351,7 +7432,7 @@
         <v>199</v>
       </c>
       <c r="E175" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F175">
         <v>0.8016737699508667</v>
@@ -7374,10 +7455,10 @@
         <v>10</v>
       </c>
       <c r="D176" t="s">
+        <v>357</v>
+      </c>
+      <c r="E176" t="s">
         <v>358</v>
-      </c>
-      <c r="E176" t="s">
-        <v>359</v>
       </c>
       <c r="F176">
         <v>0.81519734859466553</v>
@@ -7400,10 +7481,10 @@
         <v>13</v>
       </c>
       <c r="D177" t="s">
+        <v>359</v>
+      </c>
+      <c r="E177" t="s">
         <v>360</v>
-      </c>
-      <c r="E177" t="s">
-        <v>361</v>
       </c>
       <c r="F177">
         <v>0.79507380723953247</v>
@@ -7426,10 +7507,10 @@
         <v>16</v>
       </c>
       <c r="D178" t="s">
+        <v>361</v>
+      </c>
+      <c r="E178" t="s">
         <v>362</v>
-      </c>
-      <c r="E178" t="s">
-        <v>363</v>
       </c>
       <c r="F178">
         <v>0.98215627670288086</v>
@@ -7452,10 +7533,10 @@
         <v>19</v>
       </c>
       <c r="D179" t="s">
+        <v>363</v>
+      </c>
+      <c r="E179" t="s">
         <v>364</v>
-      </c>
-      <c r="E179" t="s">
-        <v>365</v>
       </c>
       <c r="F179">
         <v>0.99212384223937988</v>
@@ -7478,10 +7559,10 @@
         <v>22</v>
       </c>
       <c r="D180" t="s">
+        <v>365</v>
+      </c>
+      <c r="E180" t="s">
         <v>366</v>
-      </c>
-      <c r="E180" t="s">
-        <v>367</v>
       </c>
       <c r="F180">
         <v>0.85038471221923828</v>
@@ -7504,10 +7585,10 @@
         <v>25</v>
       </c>
       <c r="D181" t="s">
+        <v>367</v>
+      </c>
+      <c r="E181" t="s">
         <v>368</v>
-      </c>
-      <c r="E181" t="s">
-        <v>369</v>
       </c>
       <c r="F181">
         <v>0.83643585443496704</v>
@@ -7530,10 +7611,10 @@
         <v>28</v>
       </c>
       <c r="D182" t="s">
+        <v>369</v>
+      </c>
+      <c r="E182" t="s">
         <v>370</v>
-      </c>
-      <c r="E182" t="s">
-        <v>371</v>
       </c>
       <c r="F182">
         <v>0.85053074359893799</v>
@@ -7556,10 +7637,10 @@
         <v>31</v>
       </c>
       <c r="D183" t="s">
+        <v>371</v>
+      </c>
+      <c r="E183" t="s">
         <v>372</v>
-      </c>
-      <c r="E183" t="s">
-        <v>373</v>
       </c>
       <c r="F183">
         <v>0.83856010437011719</v>
@@ -7582,10 +7663,10 @@
         <v>34</v>
       </c>
       <c r="D184" t="s">
+        <v>373</v>
+      </c>
+      <c r="E184" t="s">
         <v>374</v>
-      </c>
-      <c r="E184" t="s">
-        <v>375</v>
       </c>
       <c r="F184">
         <v>0.88554084300994873</v>
@@ -7608,10 +7689,10 @@
         <v>37</v>
       </c>
       <c r="D185" t="s">
+        <v>375</v>
+      </c>
+      <c r="E185" t="s">
         <v>376</v>
-      </c>
-      <c r="E185" t="s">
-        <v>377</v>
       </c>
       <c r="F185">
         <v>0.89129257202148438</v>
@@ -7634,10 +7715,10 @@
         <v>40</v>
       </c>
       <c r="D186" t="s">
+        <v>377</v>
+      </c>
+      <c r="E186" t="s">
         <v>378</v>
-      </c>
-      <c r="E186" t="s">
-        <v>379</v>
       </c>
       <c r="F186">
         <v>0.84487235546112061</v>
@@ -7651,19 +7732,19 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B187" t="s">
         <v>331</v>
       </c>
       <c r="C187" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D187" t="s">
         <v>90</v>
       </c>
       <c r="E187" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F187">
         <v>0.85650646686553955</v>
@@ -7677,19 +7758,19 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B188" t="s">
         <v>331</v>
       </c>
       <c r="C188" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D188" t="s">
         <v>92</v>
       </c>
       <c r="E188" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F188">
         <v>0.86029088497161865</v>
@@ -7703,19 +7784,19 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B189" t="s">
         <v>331</v>
       </c>
       <c r="C189" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D189" t="s">
         <v>94</v>
       </c>
       <c r="E189" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F189">
         <v>0.83850812911987305</v>
@@ -7729,19 +7810,19 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B190" t="s">
         <v>331</v>
       </c>
       <c r="C190" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D190" t="s">
         <v>96</v>
       </c>
       <c r="E190" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F190">
         <v>0.85407382249832153</v>
@@ -7755,19 +7836,19 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B191" t="s">
         <v>331</v>
       </c>
       <c r="C191" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D191" t="s">
         <v>98</v>
       </c>
       <c r="E191" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F191">
         <v>0.83753633499145508</v>
@@ -7781,19 +7862,19 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B192" t="s">
         <v>331</v>
       </c>
       <c r="C192" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D192" t="s">
+        <v>385</v>
+      </c>
+      <c r="E192" t="s">
         <v>386</v>
-      </c>
-      <c r="E192" t="s">
-        <v>387</v>
       </c>
       <c r="F192">
         <v>0.85103440284729004</v>
@@ -7807,19 +7888,19 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B193" t="s">
         <v>331</v>
       </c>
       <c r="C193" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D193" t="s">
         <v>102</v>
       </c>
       <c r="E193" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F193">
         <v>0.86924529075622559</v>
@@ -7833,19 +7914,19 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B194" t="s">
         <v>331</v>
       </c>
       <c r="C194" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D194" t="s">
         <v>104</v>
       </c>
       <c r="E194" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F194">
         <v>0.84253275394439697</v>
@@ -7859,19 +7940,19 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B195" t="s">
         <v>331</v>
       </c>
       <c r="C195" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D195" t="s">
+        <v>389</v>
+      </c>
+      <c r="E195" t="s">
         <v>390</v>
-      </c>
-      <c r="E195" t="s">
-        <v>391</v>
       </c>
       <c r="F195">
         <v>0.83964943885803223</v>
@@ -7885,7 +7966,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B196" t="s">
         <v>331</v>
@@ -7897,7 +7978,7 @@
         <v>109</v>
       </c>
       <c r="E196" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F196">
         <v>0.8724396824836731</v>
@@ -7911,7 +7992,7 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B197" t="s">
         <v>331</v>
@@ -7923,7 +8004,7 @@
         <v>12</v>
       </c>
       <c r="E197" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F197">
         <v>0.79017913341522217</v>
@@ -7937,7 +8018,7 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B198" t="s">
         <v>331</v>
@@ -7949,7 +8030,7 @@
         <v>14</v>
       </c>
       <c r="E198" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F198">
         <v>0.81579285860061646</v>
@@ -7963,7 +8044,7 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B199" t="s">
         <v>331</v>
@@ -7975,7 +8056,7 @@
         <v>17</v>
       </c>
       <c r="E199" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F199">
         <v>0.92626184225082397</v>
@@ -7989,7 +8070,7 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B200" t="s">
         <v>331</v>
@@ -8001,7 +8082,7 @@
         <v>20</v>
       </c>
       <c r="E200" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F200">
         <v>0.8868529200553894</v>
@@ -8015,7 +8096,7 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B201" t="s">
         <v>331</v>
@@ -8027,7 +8108,7 @@
         <v>23</v>
       </c>
       <c r="E201" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F201">
         <v>0.97741824388504028</v>
@@ -8041,7 +8122,7 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B202" t="s">
         <v>331</v>
@@ -8053,7 +8134,7 @@
         <v>26</v>
       </c>
       <c r="E202" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F202">
         <v>0.83608144521713257</v>
@@ -8067,7 +8148,7 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B203" t="s">
         <v>331</v>
@@ -8079,7 +8160,7 @@
         <v>29</v>
       </c>
       <c r="E203" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F203">
         <v>0.83720672130584717</v>
@@ -8093,7 +8174,7 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B204" t="s">
         <v>331</v>
@@ -8102,10 +8183,10 @@
         <v>31</v>
       </c>
       <c r="D204" t="s">
+        <v>400</v>
+      </c>
+      <c r="E204" t="s">
         <v>401</v>
-      </c>
-      <c r="E204" t="s">
-        <v>402</v>
       </c>
       <c r="F204">
         <v>0.82314002513885498</v>
@@ -8119,7 +8200,7 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B205" t="s">
         <v>331</v>
@@ -8131,7 +8212,7 @@
         <v>35</v>
       </c>
       <c r="E205" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F205">
         <v>0.89464390277862549</v>
@@ -8145,7 +8226,7 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B206" t="s">
         <v>331</v>
@@ -8157,7 +8238,7 @@
         <v>38</v>
       </c>
       <c r="E206" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F206">
         <v>0.83675998449325562</v>
@@ -8171,7 +8252,7 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B207" t="s">
         <v>331</v>
@@ -8183,7 +8264,7 @@
         <v>41</v>
       </c>
       <c r="E207" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F207">
         <v>0.86373895406723022</v>
@@ -8197,7 +8278,7 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B208" t="s">
         <v>331</v>
@@ -8206,10 +8287,10 @@
         <v>43</v>
       </c>
       <c r="D208" t="s">
+        <v>405</v>
+      </c>
+      <c r="E208" t="s">
         <v>406</v>
-      </c>
-      <c r="E208" t="s">
-        <v>407</v>
       </c>
       <c r="F208">
         <v>0.84124410152435303</v>
@@ -8223,7 +8304,7 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B209" t="s">
         <v>331</v>
@@ -8232,10 +8313,10 @@
         <v>46</v>
       </c>
       <c r="D209" t="s">
+        <v>407</v>
+      </c>
+      <c r="E209" t="s">
         <v>408</v>
-      </c>
-      <c r="E209" t="s">
-        <v>409</v>
       </c>
       <c r="F209">
         <v>0.81275391578674316</v>
@@ -8249,7 +8330,7 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B210" t="s">
         <v>331</v>
@@ -8261,7 +8342,7 @@
         <v>50</v>
       </c>
       <c r="E210" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F210">
         <v>0.83367300033569336</v>
@@ -8275,7 +8356,7 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B211" t="s">
         <v>331</v>
@@ -8284,10 +8365,10 @@
         <v>52</v>
       </c>
       <c r="D211" t="s">
+        <v>410</v>
+      </c>
+      <c r="E211" t="s">
         <v>411</v>
-      </c>
-      <c r="E211" t="s">
-        <v>412</v>
       </c>
       <c r="F211">
         <v>0.84744298458099365</v>
@@ -8301,7 +8382,7 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B212" t="s">
         <v>9</v>
@@ -8310,10 +8391,10 @@
         <v>10</v>
       </c>
       <c r="D212" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E212" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F212">
         <v>0.7789953351020813</v>
@@ -8327,7 +8408,7 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B213" t="s">
         <v>9</v>
@@ -8336,10 +8417,10 @@
         <v>13</v>
       </c>
       <c r="D213" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E213" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F213">
         <v>0.75677555799484253</v>
@@ -8353,7 +8434,7 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B214" t="s">
         <v>9</v>
@@ -8362,10 +8443,10 @@
         <v>16</v>
       </c>
       <c r="D214" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E214" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F214">
         <v>0.79942184686660767</v>
@@ -8379,7 +8460,7 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B215" t="s">
         <v>9</v>
@@ -8388,10 +8469,10 @@
         <v>19</v>
       </c>
       <c r="D215" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E215" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F215">
         <v>0.89344584941864014</v>
@@ -8405,7 +8486,7 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B216" t="s">
         <v>9</v>
@@ -8414,10 +8495,10 @@
         <v>22</v>
       </c>
       <c r="D216" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E216" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F216">
         <v>0.85211873054504395</v>
@@ -8431,7 +8512,7 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B217" t="s">
         <v>9</v>
@@ -8440,10 +8521,10 @@
         <v>25</v>
       </c>
       <c r="D217" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E217" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F217">
         <v>0.80532276630401611</v>
@@ -8457,7 +8538,7 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B218" t="s">
         <v>9</v>
@@ -8466,10 +8547,10 @@
         <v>28</v>
       </c>
       <c r="D218" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E218" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F218">
         <v>0.81199729442596436</v>
@@ -8483,7 +8564,7 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B219" t="s">
         <v>9</v>
@@ -8492,10 +8573,10 @@
         <v>31</v>
       </c>
       <c r="D219" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E219" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F219">
         <v>0.82202422618865967</v>
@@ -8509,7 +8590,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B220" t="s">
         <v>9</v>
@@ -8518,10 +8599,10 @@
         <v>34</v>
       </c>
       <c r="D220" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E220" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F220">
         <v>0.87674158811569214</v>
@@ -8535,7 +8616,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B221" t="s">
         <v>9</v>
@@ -8544,10 +8625,10 @@
         <v>37</v>
       </c>
       <c r="D221" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E221" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F221">
         <v>0.87045812606811523</v>
@@ -8561,7 +8642,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B222" t="s">
         <v>9</v>
@@ -8570,10 +8651,10 @@
         <v>40</v>
       </c>
       <c r="D222" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E222" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F222">
         <v>0.81965172290802002</v>
@@ -8587,7 +8668,7 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B223" t="s">
         <v>9</v>
@@ -8596,10 +8677,10 @@
         <v>43</v>
       </c>
       <c r="D223" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E223" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F223">
         <v>0.79606670141220093</v>
@@ -8613,7 +8694,7 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B224" t="s">
         <v>9</v>
@@ -8622,10 +8703,10 @@
         <v>46</v>
       </c>
       <c r="D224" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E224" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F224">
         <v>0.78099387884140015</v>
@@ -8639,7 +8720,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B225" t="s">
         <v>9</v>
@@ -8648,10 +8729,10 @@
         <v>49</v>
       </c>
       <c r="D225" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E225" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F225">
         <v>0.81293618679046631</v>
@@ -8665,7 +8746,7 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>413</v>
+        <v>111</v>
       </c>
       <c r="B226" t="s">
         <v>9</v>
@@ -8674,10 +8755,10 @@
         <v>52</v>
       </c>
       <c r="D226" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E226" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F226">
         <v>0.79826062917709351</v>
@@ -8697,13 +8778,13 @@
         <v>9</v>
       </c>
       <c r="C227" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D227" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E227" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F227">
         <v>0.86863327000000001</v>
@@ -8723,13 +8804,13 @@
         <v>9</v>
       </c>
       <c r="C228" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D228" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E228" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F228">
         <v>0.81166094499999997</v>
@@ -8749,13 +8830,13 @@
         <v>9</v>
       </c>
       <c r="C229" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D229" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E229" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F229">
         <v>0.76762932500000003</v>
@@ -8775,13 +8856,13 @@
         <v>9</v>
       </c>
       <c r="C230" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D230" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E230" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F230">
         <v>0.79102379099999998</v>
@@ -8801,13 +8882,13 @@
         <v>9</v>
       </c>
       <c r="C231" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D231" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E231" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F231">
         <v>0.81073641799999996</v>
@@ -8827,13 +8908,13 @@
         <v>9</v>
       </c>
       <c r="C232" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D232" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E232" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F232">
         <v>0.81332331899999999</v>
@@ -8853,13 +8934,13 @@
         <v>9</v>
       </c>
       <c r="C233" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D233" t="s">
         <v>102</v>
       </c>
       <c r="E233" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F233">
         <v>0.78436845499999996</v>
@@ -8879,13 +8960,13 @@
         <v>9</v>
       </c>
       <c r="C234" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D234" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E234" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F234">
         <v>0.81661778699999998</v>
@@ -8905,13 +8986,13 @@
         <v>9</v>
       </c>
       <c r="C235" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D235" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E235" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F235">
         <v>0.79514116000000001</v>
@@ -8934,10 +9015,10 @@
         <v>108</v>
       </c>
       <c r="D236" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E236" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F236">
         <v>0.77562367899999995</v>
@@ -8963,16 +9044,16 @@
         <v>288</v>
       </c>
       <c r="E237" t="s">
+        <v>459</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="G237" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="F237" s="3" t="s">
+      <c r="H237" s="3" t="s">
         <v>462</v>
-      </c>
-      <c r="G237" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="H237" s="3" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
@@ -8989,16 +9070,16 @@
         <v>289</v>
       </c>
       <c r="E238" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F238" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G238">
         <v>0.80171430110931396</v>
       </c>
       <c r="H238" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
@@ -9015,16 +9096,16 @@
         <v>291</v>
       </c>
       <c r="E239" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F239" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G239">
         <v>0.91310715675354004</v>
       </c>
       <c r="H239" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
@@ -9041,13 +9122,13 @@
         <v>293</v>
       </c>
       <c r="E240" t="s">
+        <v>469</v>
+      </c>
+      <c r="F240" t="s">
+        <v>470</v>
+      </c>
+      <c r="G240" t="s">
         <v>471</v>
-      </c>
-      <c r="F240" t="s">
-        <v>472</v>
-      </c>
-      <c r="G240" t="s">
-        <v>473</v>
       </c>
       <c r="H240">
         <v>0.92757248878479004</v>
@@ -9067,16 +9148,16 @@
         <v>295</v>
       </c>
       <c r="E241" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F241">
         <v>0.90859800577163696</v>
       </c>
       <c r="G241" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H241" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
@@ -9093,16 +9174,16 @@
         <v>297</v>
       </c>
       <c r="E242" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F242" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G242">
         <v>0.83857607841491699</v>
       </c>
       <c r="H242" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -9116,19 +9197,19 @@
         <v>28</v>
       </c>
       <c r="D243" t="s">
+        <v>478</v>
+      </c>
+      <c r="E243" t="s">
+        <v>479</v>
+      </c>
+      <c r="F243" t="s">
         <v>480</v>
-      </c>
-      <c r="E243" t="s">
-        <v>481</v>
-      </c>
-      <c r="F243" t="s">
-        <v>482</v>
       </c>
       <c r="G243">
         <v>0.85378444194793701</v>
       </c>
       <c r="H243" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
@@ -9145,16 +9226,16 @@
         <v>301</v>
       </c>
       <c r="E244" t="s">
+        <v>482</v>
+      </c>
+      <c r="F244" t="s">
+        <v>483</v>
+      </c>
+      <c r="G244" t="s">
         <v>484</v>
       </c>
-      <c r="F244" t="s">
+      <c r="H244" t="s">
         <v>485</v>
-      </c>
-      <c r="G244" t="s">
-        <v>486</v>
-      </c>
-      <c r="H244" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
@@ -9168,19 +9249,19 @@
         <v>34</v>
       </c>
       <c r="D245" t="s">
+        <v>486</v>
+      </c>
+      <c r="E245" t="s">
+        <v>487</v>
+      </c>
+      <c r="F245" t="s">
         <v>488</v>
       </c>
-      <c r="E245" t="s">
+      <c r="G245" t="s">
         <v>489</v>
       </c>
-      <c r="F245" t="s">
+      <c r="H245" t="s">
         <v>490</v>
-      </c>
-      <c r="G245" t="s">
-        <v>491</v>
-      </c>
-      <c r="H245" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
@@ -9197,16 +9278,16 @@
         <v>305</v>
       </c>
       <c r="E246" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F246" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G246">
         <v>0.911385178565979</v>
       </c>
       <c r="H246" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.3">
@@ -9220,19 +9301,19 @@
         <v>40</v>
       </c>
       <c r="D247" t="s">
+        <v>494</v>
+      </c>
+      <c r="E247" t="s">
+        <v>495</v>
+      </c>
+      <c r="F247" t="s">
         <v>496</v>
       </c>
-      <c r="E247" t="s">
+      <c r="G247" t="s">
         <v>497</v>
       </c>
-      <c r="F247" t="s">
+      <c r="H247" t="s">
         <v>498</v>
-      </c>
-      <c r="G247" t="s">
-        <v>499</v>
-      </c>
-      <c r="H247" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.3">
@@ -9246,19 +9327,19 @@
         <v>43</v>
       </c>
       <c r="D248" t="s">
+        <v>499</v>
+      </c>
+      <c r="E248" t="s">
+        <v>500</v>
+      </c>
+      <c r="F248" t="s">
         <v>501</v>
       </c>
-      <c r="E248" t="s">
+      <c r="G248" t="s">
         <v>502</v>
       </c>
-      <c r="F248" t="s">
+      <c r="H248" t="s">
         <v>503</v>
-      </c>
-      <c r="G248" t="s">
-        <v>504</v>
-      </c>
-      <c r="H248" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.3">
@@ -9272,19 +9353,19 @@
         <v>46</v>
       </c>
       <c r="D249" t="s">
+        <v>504</v>
+      </c>
+      <c r="E249" t="s">
+        <v>505</v>
+      </c>
+      <c r="F249" t="s">
         <v>506</v>
       </c>
-      <c r="E249" t="s">
+      <c r="G249" t="s">
         <v>507</v>
       </c>
-      <c r="F249" t="s">
+      <c r="H249" t="s">
         <v>508</v>
-      </c>
-      <c r="G249" t="s">
-        <v>509</v>
-      </c>
-      <c r="H249" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.3">
@@ -9298,19 +9379,19 @@
         <v>49</v>
       </c>
       <c r="D250" t="s">
+        <v>509</v>
+      </c>
+      <c r="E250" t="s">
+        <v>510</v>
+      </c>
+      <c r="F250" t="s">
         <v>511</v>
       </c>
-      <c r="E250" t="s">
+      <c r="G250" t="s">
         <v>512</v>
       </c>
-      <c r="F250" t="s">
+      <c r="H250" t="s">
         <v>513</v>
-      </c>
-      <c r="G250" t="s">
-        <v>514</v>
-      </c>
-      <c r="H250" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.3">
@@ -9324,24 +9405,166 @@
         <v>52</v>
       </c>
       <c r="D251" t="s">
+        <v>514</v>
+      </c>
+      <c r="E251" t="s">
+        <v>515</v>
+      </c>
+      <c r="F251" t="s">
         <v>516</v>
       </c>
-      <c r="E251" t="s">
+      <c r="G251" t="s">
         <v>517</v>
       </c>
-      <c r="F251" t="s">
+      <c r="H251" t="s">
         <v>518</v>
       </c>
-      <c r="G251" t="s">
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>231</v>
+      </c>
+      <c r="B252" t="s">
+        <v>331</v>
+      </c>
+      <c r="C252" t="s">
+        <v>52</v>
+      </c>
+      <c r="D252" t="s">
         <v>519</v>
       </c>
-      <c r="H251" t="s">
+      <c r="E252" t="s">
         <v>520</v>
       </c>
+      <c r="F252">
+        <v>0.82585513591766357</v>
+      </c>
+      <c r="G252">
+        <v>0.84710931777954102</v>
+      </c>
+      <c r="H252">
+        <v>0.83634722232818604</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>111</v>
+      </c>
+      <c r="B253" t="s">
+        <v>331</v>
+      </c>
+      <c r="C253" t="s">
+        <v>43</v>
+      </c>
+      <c r="D253" t="s">
+        <v>423</v>
+      </c>
+      <c r="E253" t="s">
+        <v>521</v>
+      </c>
+      <c r="F253">
+        <v>0.81666189432144165</v>
+      </c>
+      <c r="G253">
+        <v>0.83901494741439819</v>
+      </c>
+      <c r="H253">
+        <v>0.82768750190734863</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>111</v>
+      </c>
+      <c r="B254" t="s">
+        <v>331</v>
+      </c>
+      <c r="C254" t="s">
+        <v>46</v>
+      </c>
+      <c r="D254" t="s">
+        <v>522</v>
+      </c>
+      <c r="E254" t="s">
+        <v>523</v>
+      </c>
+      <c r="F254">
+        <v>0.82013803720474243</v>
+      </c>
+      <c r="G254">
+        <v>0.8417133092880249</v>
+      </c>
+      <c r="H254">
+        <v>0.83078557252883911</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>111</v>
+      </c>
+      <c r="B255" t="s">
+        <v>331</v>
+      </c>
+      <c r="C255" t="s">
+        <v>49</v>
+      </c>
+      <c r="D255" t="s">
+        <v>427</v>
+      </c>
+      <c r="E255" t="s">
+        <v>524</v>
+      </c>
+      <c r="F255">
+        <v>0.83635401725769043</v>
+      </c>
+      <c r="G255">
+        <v>0.8642503023147583</v>
+      </c>
+      <c r="H255">
+        <v>0.85007333755493164</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>111</v>
+      </c>
+      <c r="B256" t="s">
+        <v>331</v>
+      </c>
+      <c r="C256" t="s">
+        <v>52</v>
+      </c>
+      <c r="D256" t="s">
+        <v>429</v>
+      </c>
+      <c r="E256" t="s">
+        <v>525</v>
+      </c>
+      <c r="F256">
+        <v>0.81242471933364868</v>
+      </c>
+      <c r="G256">
+        <v>0.86384886503219604</v>
+      </c>
+      <c r="H256">
+        <v>0.83734798431396484</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H236" xr:uid="{B0490D49-417E-4222-A93E-5008B1C77A87}"/>
+  <autoFilter ref="A1:H256" xr:uid="{B0490D49-417E-4222-A93E-5008B1C77A87}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D252:H252">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D253:H253">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D254:H254">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D255:H256">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9433,47 +9656,47 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -9483,12 +9706,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>